<commit_message>
Added Re-test Results in testcases file
</commit_message>
<xml_diff>
--- a/1-Testing of the App/City Social TEST Plan & Cases.xlsx
+++ b/1-Testing of the App/City Social TEST Plan & Cases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A9DA33-F2ED-4636-A0FB-113192A73022}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07E1178-5A8F-422E-A6F3-0EA17318B2E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
   <si>
     <t>Test cases</t>
   </si>
@@ -319,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +407,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -603,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -668,6 +681,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -704,12 +720,24 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -736,6 +764,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,13 +1067,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="20" t="s">
         <v>43</v>
       </c>
@@ -1060,10 +1091,10 @@
       <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="41"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="14"/>
       <c r="G2" s="15"/>
       <c r="H2" s="16"/>
@@ -1092,18 +1123,18 @@
       <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="44"/>
+      <c r="J4" s="49"/>
     </row>
     <row r="5" spans="1:10" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
@@ -1118,18 +1149,18 @@
       <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28" t="s">
+      <c r="H5" s="28"/>
+      <c r="I5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="28"/>
+      <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
@@ -1144,18 +1175,18 @@
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="33" t="s">
+      <c r="H6" s="28"/>
+      <c r="I6" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J6" s="33"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
@@ -1170,18 +1201,18 @@
       <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27" t="s">
+      <c r="F7" s="27"/>
+      <c r="G7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="33" t="s">
+      <c r="H7" s="28"/>
+      <c r="I7" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="33"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
@@ -1196,18 +1227,18 @@
       <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="33"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
@@ -1222,38 +1253,38 @@
       <c r="D9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="27" t="s">
+      <c r="F9" s="27"/>
+      <c r="G9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="33" t="s">
+      <c r="H9" s="28"/>
+      <c r="I9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="33"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>6</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="11"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="27" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="33" t="s">
+      <c r="H10" s="28"/>
+      <c r="I10" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="33"/>
+      <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
@@ -1268,24 +1299,24 @@
       <c r="D11" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28" t="s">
+      <c r="H11" s="28"/>
+      <c r="I11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="28"/>
+      <c r="J11" s="29"/>
     </row>
     <row r="12" spans="1:10" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1294,18 +1325,18 @@
       <c r="D12" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="29" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="30"/>
-      <c r="I12" s="28" t="s">
+      <c r="H12" s="31"/>
+      <c r="I12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="28"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
@@ -1320,18 +1351,18 @@
       <c r="D13" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="29"/>
     </row>
     <row r="14" spans="1:10" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
@@ -1346,18 +1377,18 @@
       <c r="D14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="33" t="s">
+      <c r="H14" s="28"/>
+      <c r="I14" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J14" s="33"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
@@ -1372,18 +1403,18 @@
       <c r="D15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27" t="s">
+      <c r="F15" s="27"/>
+      <c r="G15" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="33" t="s">
+      <c r="H15" s="28"/>
+      <c r="I15" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="33"/>
+      <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
@@ -1396,16 +1427,16 @@
         <v>40</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28" t="s">
+      <c r="H16" s="28"/>
+      <c r="I16" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="28"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
@@ -1420,24 +1451,24 @@
       <c r="D17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27" t="s">
+      <c r="F17" s="27"/>
+      <c r="G17" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>14</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1446,21 +1477,21 @@
       <c r="D18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27" t="s">
+      <c r="F18" s="27"/>
+      <c r="G18" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="33" t="s">
+      <c r="H18" s="28"/>
+      <c r="I18" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="33"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22">
+      <c r="A19" s="23">
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1472,24 +1503,24 @@
       <c r="D19" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="29" t="s">
+      <c r="F19" s="27"/>
+      <c r="G19" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="34" t="s">
+      <c r="H19" s="41"/>
+      <c r="I19" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="35"/>
+      <c r="J19" s="39"/>
     </row>
     <row r="20" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>16</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="24" t="s">
         <v>59</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1498,24 +1529,24 @@
       <c r="D20" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28" t="s">
+      <c r="H20" s="28"/>
+      <c r="I20" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="28"/>
+      <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>17</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="24" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -1524,24 +1555,24 @@
       <c r="D21" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28" t="s">
+      <c r="H21" s="28"/>
+      <c r="I21" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="28"/>
+      <c r="J21" s="29"/>
     </row>
     <row r="22" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>18</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1550,24 +1581,24 @@
       <c r="D22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27" t="s">
+      <c r="F22" s="27"/>
+      <c r="G22" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28" t="s">
+      <c r="H22" s="28"/>
+      <c r="I22" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="28"/>
+      <c r="J22" s="29"/>
     </row>
     <row r="23" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="24" t="s">
         <v>73</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -1576,87 +1607,200 @@
       <c r="D23" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27" t="s">
+      <c r="F23" s="27"/>
+      <c r="G23" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="33" t="s">
+      <c r="H23" s="28"/>
+      <c r="I23" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J23" s="33"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-    </row>
-    <row r="28" spans="1:10" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+    </row>
+    <row r="26" spans="1:10" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>20</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="28"/>
+      <c r="I26" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>21</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="28"/>
+      <c r="I27" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J27" s="29"/>
+    </row>
+    <row r="28" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>22</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="37"/>
+      <c r="G28" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="31"/>
+      <c r="I28" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="J28" s="39"/>
+    </row>
+    <row r="29" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>23</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="40"/>
+      <c r="G29" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="28"/>
+      <c r="I29" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>24</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="35"/>
+      <c r="G30" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="28"/>
+      <c r="I30" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>25</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="28"/>
+      <c r="I31" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="81">
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="E4:F4"/>
@@ -1701,6 +1845,21 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:J20"/>

</xml_diff>